<commit_message>
Melhorado erro na pagina do excel e melhorias no filtro avançado
</commit_message>
<xml_diff>
--- a/storage/app/public/uploads/Modelo_Dados.xlsx
+++ b/storage/app/public/uploads/Modelo_Dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156DABB1-8B67-4651-AAA9-91B6EFF2BC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43F71F9B-9FBB-4269-89AB-5B09E88C6DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CFCAA012-CB54-4BDC-8065-AD85713840AD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Setor</t>
   </si>
@@ -61,46 +61,16 @@
   </si>
   <si>
     <t>DataPlantio</t>
-  </si>
-  <si>
-    <t>Fazenda-teste</t>
-  </si>
-  <si>
-    <t>IACSP90-4039</t>
-  </si>
-  <si>
-    <t>1AM</t>
-  </si>
-  <si>
-    <t>20.01</t>
-  </si>
-  <si>
-    <t>2AM</t>
-  </si>
-  <si>
-    <t>15.67</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF212529"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,10 +96,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,8 +116,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B037985D-F576-48A3-9C63-7799AA7347F1}" name="Tabela1" displayName="Tabela1" ref="A1:H3" totalsRowShown="0">
-  <autoFilter ref="A1:H3" xr:uid="{B037985D-F576-48A3-9C63-7799AA7347F1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B037985D-F576-48A3-9C63-7799AA7347F1}" name="Tabela1" displayName="Tabela1" ref="A1:H2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{B037985D-F576-48A3-9C63-7799AA7347F1}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{D4BE9656-5E19-4383-A822-EDB62A0E9579}" name="Setor"/>
     <tableColumn id="2" xr3:uid="{23DB716C-046B-4D09-A77A-812B4EA29AEF}" name="Fazenda"/>
@@ -461,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB01BB8-40AE-4299-9AFC-F8A271ADBF32}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,64 +473,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1234</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>45941</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1234</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>45911</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>